<commit_message>
build CR on top of SMRLv6
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_itemshape_1/Bugzilla_list.xlsx
+++ b/publication/part1000/CR_itemshape_1/Bugzilla_list.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/AP242Ed2/CRandCD/CR_itemshape_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klt/Projets/EclipseWS_CR_itemshape1/stepmod/publication/part1000/CR_itemshape_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Geometry" sheetId="2" r:id="rId2"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
+    <sheet name="Geometry_1" sheetId="2" r:id="rId2"/>
+    <sheet name="Itemshape_1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="343">
   <si>
     <t>d</t>
   </si>
@@ -961,13 +962,112 @@
   </si>
   <si>
     <t>5425</t>
+  </si>
+  <si>
+    <t>5468</t>
+  </si>
+  <si>
+    <t>product_view_definition</t>
+  </si>
+  <si>
+    <t>assembly_structure</t>
+  </si>
+  <si>
+    <t>contextual_shape_positioning</t>
+  </si>
+  <si>
+    <t>part nb</t>
+  </si>
+  <si>
+    <t>part name</t>
+  </si>
+  <si>
+    <t>1802</t>
+  </si>
+  <si>
+    <t>assembly_component</t>
+  </si>
+  <si>
+    <t>1808</t>
+  </si>
+  <si>
+    <t>assembly_shape</t>
+  </si>
+  <si>
+    <t>1026</t>
+  </si>
+  <si>
+    <t>1311</t>
+  </si>
+  <si>
+    <t>associative_draughting_elements</t>
+  </si>
+  <si>
+    <t>1765</t>
+  </si>
+  <si>
+    <t>characterizable_object</t>
+  </si>
+  <si>
+    <t>1809</t>
+  </si>
+  <si>
+    <t>default_setting_association</t>
+  </si>
+  <si>
+    <t>1232</t>
+  </si>
+  <si>
+    <t>design_material_aspects</t>
+  </si>
+  <si>
+    <t>1815</t>
+  </si>
+  <si>
+    <t>mating_structure</t>
+  </si>
+  <si>
+    <t>1816</t>
+  </si>
+  <si>
+    <t>model_based_3d_geometrical_dimensioning_and_tolerancing_representation</t>
+  </si>
+  <si>
+    <t>1019</t>
+  </si>
+  <si>
+    <t>1041</t>
+  </si>
+  <si>
+    <t>product_view_definition_relationship</t>
+  </si>
+  <si>
+    <t>1524</t>
+  </si>
+  <si>
+    <t>shape_data_quality_inspection_result</t>
+  </si>
+  <si>
+    <t>1764</t>
+  </si>
+  <si>
+    <t>shape_feature</t>
+  </si>
+  <si>
+    <t>shape_property_assignment</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>surface_conditions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -994,8 +1094,16 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1013,8 +1121,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1050,12 +1170,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1110,6 +1256,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -1649,9 +1801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K155" sqref="K155"/>
+      <selection pane="bottomLeft" activeCell="K127" sqref="K127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3414,8 +3566,8 @@
         <v>298</v>
       </c>
       <c r="J74" s="5"/>
-      <c r="K74" s="4">
-        <v>5468</v>
+      <c r="K74" s="4" t="s">
+        <v>310</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>84</v>
@@ -5625,4 +5777,158 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="59.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
version used for today build
</commit_message>
<xml_diff>
--- a/publication/part1000/CR_itemshape_1/Bugzilla_list.xlsx
+++ b/publication/part1000/CR_itemshape_1/Bugzilla_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,6 +16,9 @@
     <sheet name="Geometry_1" sheetId="2" r:id="rId2"/>
     <sheet name="Itemshape_1" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Itemshape_1!$A$1:$B$17</definedName>
+  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1067,7 +1070,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1098,6 +1101,22 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1197,9 +1216,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1263,7 +1284,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5784,7 +5807,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5802,133 +5825,138 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>316</v>
+        <v>333</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>319</v>
+      <c r="A3" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>320</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>312</v>
+      <c r="A4" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
-        <v>321</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>322</v>
+      <c r="A5" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>323</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>324</v>
+      <c r="A6" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
-        <v>200</v>
+        <v>341</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>313</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>325</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>326</v>
+      <c r="A8" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>311</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="24" t="s">
-        <v>334</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>335</v>
+      <c r="A13" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>337</v>
+      <c r="A14" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="24" t="s">
-        <v>338</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>339</v>
+      <c r="A15" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>189</v>
+        <v>329</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B17">
+    <sortState ref="A2:B17">
+      <sortCondition ref="A1:A17"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>